<commit_message>
AW calculations for growth
</commit_message>
<xml_diff>
--- a/2.Growth/New_BW.xlsx
+++ b/2.Growth/New_BW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ana.maria.palacio/Documents/Projects_RSMAS/2017-Nutrients/Nutrients_Caribbean/2.Growth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677BC76A-604C-7242-B347-9E523F41F2FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F9AAFE-AE0C-DB40-BA41-E12B45C57BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22300" yWindow="-1340" windowWidth="27240" windowHeight="16440" xr2:uid="{C54378E0-41F9-0B44-91E6-9486B248C99B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2470" uniqueCount="84">
   <si>
     <t>Fragment</t>
   </si>
@@ -278,6 +278,12 @@
   <si>
     <t>W_density</t>
   </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>AW</t>
+  </si>
 </sst>
 </file>
 
@@ -288,7 +294,7 @@
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -353,6 +359,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD0BF69"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -374,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,6 +406,7 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,7 +724,7 @@
   <dimension ref="A1:DA147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -747,7 +760,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>9</v>
@@ -764,7 +777,9 @@
       <c r="N1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="3"/>
+      <c r="O1" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="1" t="s">
@@ -1063,7 +1078,10 @@
         <f xml:space="preserve"> K2 + (L2*G2) + M2*G2^(3/2) + 0.00048314*G2^2</f>
         <v>1021.8431267740447</v>
       </c>
-      <c r="O2" s="3"/>
+      <c r="O2" s="19">
+        <f>I2*(1/     (1-   (0.001*N2/1.84)))</f>
+        <v>6.220616322555073</v>
+      </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="1"/>
@@ -1200,6 +1218,10 @@
         <f t="shared" ref="N3:N66" si="0" xml:space="preserve"> K3 + (L3*G3) + M3*G3^(3/2) + 0.00048314*G3^2</f>
         <v>1021.1617293120976</v>
       </c>
+      <c r="O3" s="19">
+        <f t="shared" ref="O3:O66" si="1">I3*(1/     (1-   (0.001*N3/1.84)))</f>
+        <v>5.6671508478732342</v>
+      </c>
       <c r="R3" s="9">
         <v>43026</v>
       </c>
@@ -1487,20 +1509,24 @@
         <v>42</v>
       </c>
       <c r="K4" s="12">
-        <f t="shared" ref="K4:K67" si="1">1000*(1-(F4+288.9414)/(508929.2*(F4+68.12963))*(F4-3.9863)^2)</f>
+        <f t="shared" ref="K4:K67" si="2">1000*(1-(F4+288.9414)/(508929.2*(F4+68.12963))*(F4-3.9863)^2)</f>
         <v>997.25217771670884</v>
       </c>
       <c r="L4" s="15">
-        <f t="shared" ref="L4:L67" si="2" xml:space="preserve"> 0.824493 - 0.0040899*F4 + 0.000076438*F4^2 -0.00000082467*F4^3 + 0.0000000053675*F4^4</f>
+        <f t="shared" ref="L4:L67" si="3" xml:space="preserve"> 0.824493 - 0.0040899*F4 + 0.000076438*F4^2 -0.00000082467*F4^3 + 0.0000000053675*F4^4</f>
         <v>0.76028272301154676</v>
       </c>
       <c r="M4" s="17">
-        <f t="shared" ref="M4:M67" si="3" xml:space="preserve"> -0.005724 + 0.00010227*F4 - 0.0000016546*F4^2</f>
+        <f t="shared" ref="M4:M67" si="4" xml:space="preserve"> -0.005724 + 0.00010227*F4 - 0.0000016546*F4^2</f>
         <v>-4.2158637539999998E-3</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
         <v>1021.1617293120976</v>
+      </c>
+      <c r="O4" s="19">
+        <f t="shared" si="1"/>
+        <v>7.1861809720454417</v>
       </c>
       <c r="R4" s="9">
         <v>43026</v>
@@ -1749,20 +1775,24 @@
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L5" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M5" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O5" s="19">
+        <f t="shared" si="1"/>
+        <v>4.0175632485398829</v>
       </c>
       <c r="R5" s="9">
         <v>43026</v>
@@ -2011,20 +2041,24 @@
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L6" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M6" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
         <v>1021.2612205430163</v>
+      </c>
+      <c r="O6" s="19">
+        <f t="shared" si="1"/>
+        <v>6.5712778422054345</v>
       </c>
       <c r="R6" s="9">
         <v>43026</v>
@@ -2273,20 +2307,24 @@
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L7" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M7" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
         <v>1020.7320327829005</v>
+      </c>
+      <c r="O7" s="19">
+        <f t="shared" si="1"/>
+        <v>2.4076127456809364</v>
       </c>
       <c r="R7" s="9">
         <v>43026</v>
@@ -2571,20 +2609,24 @@
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L8" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M8" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
         <v>1021.0985005999307</v>
+      </c>
+      <c r="O8" s="19">
+        <f t="shared" si="1"/>
+        <v>3.4535044838382438</v>
       </c>
       <c r="R8" s="9">
         <v>43026</v>
@@ -2869,20 +2911,24 @@
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L9" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
         <v>1021.0229352475681</v>
+      </c>
+      <c r="O9" s="19">
+        <f t="shared" si="1"/>
+        <v>5.9515219775701622</v>
       </c>
       <c r="R9" s="9">
         <v>43026</v>
@@ -3167,20 +3213,24 @@
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L10" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M10" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N10">
         <f t="shared" si="0"/>
         <v>1021.0229352475681</v>
+      </c>
+      <c r="O10" s="19">
+        <f t="shared" si="1"/>
+        <v>5.7897592058128762</v>
       </c>
       <c r="R10" s="9">
         <v>43026</v>
@@ -3467,20 +3517,24 @@
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L11" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M11" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N11">
         <f t="shared" si="0"/>
         <v>1020.7320327829005</v>
+      </c>
+      <c r="O11" s="19">
+        <f t="shared" si="1"/>
+        <v>5.8955069565414719</v>
       </c>
       <c r="R11" s="9">
         <v>43026</v>
@@ -3765,20 +3819,24 @@
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L12" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M12" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N12">
         <f t="shared" si="0"/>
         <v>1020.7320327829005</v>
+      </c>
+      <c r="O12" s="19">
+        <f t="shared" si="1"/>
+        <v>4.1032728417528643</v>
       </c>
       <c r="R12" s="9">
         <v>43026</v>
@@ -4063,20 +4121,24 @@
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L13" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M13" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
         <v>1020.9644870534015</v>
+      </c>
+      <c r="O13" s="19">
+        <f t="shared" si="1"/>
+        <v>7.5236786471330657</v>
       </c>
       <c r="R13" s="9">
         <v>43026</v>
@@ -4361,20 +4423,24 @@
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L14" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M14" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
         <v>1020.9644870534015</v>
+      </c>
+      <c r="O14" s="19">
+        <f t="shared" si="1"/>
+        <v>9.8645783635596569</v>
       </c>
       <c r="R14" s="9">
         <v>43026</v>
@@ -4659,20 +4725,24 @@
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.25217771670884</v>
       </c>
       <c r="L15" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76028272301154676</v>
       </c>
       <c r="M15" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2158637539999998E-3</v>
       </c>
       <c r="N15">
         <f t="shared" si="0"/>
         <v>1021.1617293120976</v>
+      </c>
+      <c r="O15" s="19">
+        <f t="shared" si="1"/>
+        <v>9.750106078081668</v>
       </c>
       <c r="R15" s="9">
         <v>43026</v>
@@ -4959,20 +5029,24 @@
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L16" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M16" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N16">
         <f t="shared" si="0"/>
         <v>1021.4008023889601</v>
+      </c>
+      <c r="O16" s="19">
+        <f t="shared" si="1"/>
+        <v>5.7317427303775821</v>
       </c>
       <c r="R16" s="9">
         <v>43026</v>
@@ -5257,20 +5331,24 @@
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.35123703333397</v>
       </c>
       <c r="L17" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76089952447632669</v>
       </c>
       <c r="M17" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2248710660000004E-3</v>
       </c>
       <c r="N17">
         <f t="shared" si="0"/>
         <v>1021.3543787243402</v>
+      </c>
+      <c r="O17" s="19">
+        <f t="shared" si="1"/>
+        <v>6.113512208373189</v>
       </c>
       <c r="R17" s="9">
         <v>43026</v>
@@ -5555,20 +5633,24 @@
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L18" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M18" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N18">
         <f t="shared" si="0"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O18" s="19">
+        <f t="shared" si="1"/>
+        <v>3.1727065475046503</v>
       </c>
       <c r="R18" s="9">
         <v>43026</v>
@@ -5855,20 +5937,24 @@
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L19" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M19" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N19">
         <f t="shared" si="0"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O19" s="19">
+        <f t="shared" si="1"/>
+        <v>3.2176457337299289</v>
       </c>
       <c r="R19" s="9">
         <v>43026</v>
@@ -6153,20 +6239,24 @@
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.35123703333397</v>
       </c>
       <c r="L20" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76089952447632669</v>
       </c>
       <c r="M20" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2248710660000004E-3</v>
       </c>
       <c r="N20">
         <f t="shared" si="0"/>
         <v>1021.2787876796716</v>
+      </c>
+      <c r="O20" s="19">
+        <f t="shared" si="1"/>
+        <v>5.348829289018858</v>
       </c>
       <c r="R20" s="9">
         <v>43026</v>
@@ -6451,20 +6541,24 @@
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L21" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M21" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N21">
         <f t="shared" si="0"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O21" s="19">
+        <f t="shared" si="1"/>
+        <v>10.165243924157959</v>
       </c>
       <c r="R21" s="9">
         <v>43026</v>
@@ -6749,20 +6843,24 @@
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L22" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M22" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N22">
         <f t="shared" si="0"/>
         <v>1021.0985005999307</v>
+      </c>
+      <c r="O22" s="19">
+        <f t="shared" si="1"/>
+        <v>6.614910345100709</v>
       </c>
       <c r="R22" s="9">
         <v>43026</v>
@@ -7047,20 +7145,24 @@
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.35123703333397</v>
       </c>
       <c r="L23" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76089952447632669</v>
       </c>
       <c r="M23" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2248710660000004E-3</v>
       </c>
       <c r="N23">
         <f t="shared" si="0"/>
         <v>1021.2787876796716</v>
+      </c>
+      <c r="O23" s="19">
+        <f t="shared" si="1"/>
+        <v>7.2928365726328552</v>
       </c>
       <c r="R23" s="9">
         <v>43026</v>
@@ -7345,20 +7447,24 @@
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L24" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M24" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N24">
         <f t="shared" si="0"/>
         <v>1021.2612205430163</v>
+      </c>
+      <c r="O24" s="19">
+        <f t="shared" si="1"/>
+        <v>9.8659061994807988</v>
       </c>
       <c r="R24" s="9">
         <v>43026</v>
@@ -7645,20 +7751,24 @@
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L25" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M25" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N25">
         <f t="shared" si="0"/>
         <v>1021.2612205430163</v>
+      </c>
+      <c r="O25" s="19">
+        <f t="shared" si="1"/>
+        <v>8.7714423454609491</v>
       </c>
       <c r="R25" s="9">
         <v>43026</v>
@@ -7943,20 +8053,24 @@
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.25217771670884</v>
       </c>
       <c r="L26" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76028272301154676</v>
       </c>
       <c r="M26" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2158637539999998E-3</v>
       </c>
       <c r="N26">
         <f t="shared" si="0"/>
         <v>1021.0861963783011</v>
+      </c>
+      <c r="O26" s="19">
+        <f t="shared" si="1"/>
+        <v>6.4418012941896148</v>
       </c>
       <c r="R26" s="9">
         <v>43026</v>
@@ -8241,20 +8355,24 @@
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M27" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N27">
         <f t="shared" si="0"/>
         <v>1021.4008023889601</v>
+      </c>
+      <c r="O27" s="19">
+        <f t="shared" si="1"/>
+        <v>6.979239677577409</v>
       </c>
       <c r="R27" s="9">
         <v>43026</v>
@@ -8539,20 +8657,24 @@
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L28" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M28" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N28">
         <f t="shared" si="0"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O28" s="19">
+        <f t="shared" si="1"/>
+        <v>8.3047616144314365</v>
       </c>
       <c r="R28" s="9">
         <v>43026</v>
@@ -8839,20 +8961,24 @@
         <v>42</v>
       </c>
       <c r="K29" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L29" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M29" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N29">
         <f t="shared" si="0"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O29" s="19">
+        <f t="shared" si="1"/>
+        <v>3.4468355834788484</v>
       </c>
       <c r="R29" s="9">
         <v>43026</v>
@@ -9133,20 +9259,24 @@
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L30" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M30" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N30">
         <f t="shared" si="0"/>
         <v>1021.2612205430163</v>
+      </c>
+      <c r="O30" s="19">
+        <f t="shared" si="1"/>
+        <v>4.9644161263446671</v>
       </c>
       <c r="R30" s="9">
         <v>43026</v>
@@ -9413,20 +9543,24 @@
       </c>
       <c r="J31" s="8"/>
       <c r="K31" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L31" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M31" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N31">
         <f t="shared" si="0"/>
         <v>1021.0985005999307</v>
+      </c>
+      <c r="O31" s="19">
+        <f t="shared" si="1"/>
+        <v>8.5225390417686793</v>
       </c>
       <c r="R31" s="9">
         <v>43026</v>
@@ -9709,20 +9843,24 @@
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L32" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M32" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N32">
         <f t="shared" si="0"/>
         <v>1021.0229352475681</v>
+      </c>
+      <c r="O32" s="19">
+        <f t="shared" si="1"/>
+        <v>6.5626257819865774</v>
       </c>
       <c r="R32" s="9">
         <v>43026</v>
@@ -10009,20 +10147,24 @@
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L33" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M33" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N33">
         <f t="shared" si="0"/>
         <v>1021.4008023889601</v>
+      </c>
+      <c r="O33" s="19">
+        <f t="shared" si="1"/>
+        <v>7.3276397258944774</v>
       </c>
       <c r="R33" s="9">
         <v>43026</v>
@@ -10305,20 +10447,24 @@
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L34" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M34" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N34">
         <f t="shared" si="0"/>
         <v>1020.7320327829005</v>
+      </c>
+      <c r="O34" s="19">
+        <f t="shared" si="1"/>
+        <v>3.2385984881267817</v>
       </c>
       <c r="R34" s="9">
         <v>43026</v>
@@ -10601,20 +10747,24 @@
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L35" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M35" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N35">
         <f t="shared" si="0"/>
         <v>1020.7320327829005</v>
+      </c>
+      <c r="O35" s="19">
+        <f t="shared" si="1"/>
+        <v>11.46086552351662</v>
       </c>
       <c r="R35" s="9">
         <v>43026</v>
@@ -10897,20 +11047,24 @@
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L36" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M36" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N36">
         <f t="shared" si="0"/>
         <v>1020.9644870534015</v>
+      </c>
+      <c r="O36" s="19">
+        <f t="shared" si="1"/>
+        <v>5.3602559725468781</v>
       </c>
       <c r="R36" s="9">
         <v>43026</v>
@@ -11193,20 +11347,24 @@
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L37" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M37" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N37">
         <f t="shared" si="0"/>
         <v>1020.9644870534015</v>
+      </c>
+      <c r="O37" s="19">
+        <f t="shared" si="1"/>
+        <v>8.9884258785247528</v>
       </c>
       <c r="R37" s="9">
         <v>43026</v>
@@ -11489,20 +11647,24 @@
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.25217771670884</v>
       </c>
       <c r="L38" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76028272301154676</v>
       </c>
       <c r="M38" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2158637539999998E-3</v>
       </c>
       <c r="N38">
         <f t="shared" si="0"/>
         <v>1021.1617293120976</v>
+      </c>
+      <c r="O38" s="19">
+        <f t="shared" si="1"/>
+        <v>8.4557845521597859</v>
       </c>
       <c r="R38" s="9">
         <v>43026</v>
@@ -11785,20 +11947,24 @@
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.35123703333397</v>
       </c>
       <c r="L39" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76089952447632669</v>
       </c>
       <c r="M39" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2248710660000004E-3</v>
       </c>
       <c r="N39">
         <f t="shared" si="0"/>
         <v>1021.3543787243402</v>
+      </c>
+      <c r="O39" s="19">
+        <f t="shared" si="1"/>
+        <v>7.7947280656758151</v>
       </c>
       <c r="R39" s="9">
         <v>43026</v>
@@ -12083,20 +12249,24 @@
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.35123703333397</v>
       </c>
       <c r="L40" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76089952447632669</v>
       </c>
       <c r="M40" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2248710660000004E-3</v>
       </c>
       <c r="N40">
         <f t="shared" si="0"/>
         <v>1021.3543787243402</v>
+      </c>
+      <c r="O40" s="19">
+        <f t="shared" si="1"/>
+        <v>9.1522873942998615</v>
       </c>
       <c r="R40" s="9">
         <v>43026</v>
@@ -12383,20 +12553,24 @@
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L41" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M41" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N41">
         <f t="shared" si="0"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O41" s="19">
+        <f t="shared" si="1"/>
+        <v>2.8244278542587433</v>
       </c>
       <c r="R41" s="9">
         <v>43026</v>
@@ -12681,20 +12855,24 @@
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L42" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M42" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N42">
         <f t="shared" si="0"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O42" s="19">
+        <f t="shared" si="1"/>
+        <v>8.4800244407100216</v>
       </c>
       <c r="R42" s="9">
         <v>43026</v>
@@ -12981,20 +13159,24 @@
       </c>
       <c r="J43" s="8"/>
       <c r="K43" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.35123703333397</v>
       </c>
       <c r="L43" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76089952447632669</v>
       </c>
       <c r="M43" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2248710660000004E-3</v>
       </c>
       <c r="N43">
         <f t="shared" si="0"/>
         <v>1021.2787876796716</v>
+      </c>
+      <c r="O43" s="19">
+        <f t="shared" si="1"/>
+        <v>4.6948337751094096</v>
       </c>
       <c r="R43" s="9">
         <v>43026</v>
@@ -13271,20 +13453,24 @@
       </c>
       <c r="J44" s="8"/>
       <c r="K44" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L44" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M44" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N44">
         <f t="shared" si="0"/>
         <v>1021.3252208670636</v>
+      </c>
+      <c r="O44" s="19">
+        <f t="shared" si="1"/>
+        <v>3.2746581039657006</v>
       </c>
       <c r="R44" s="9">
         <v>43026</v>
@@ -13553,20 +13739,24 @@
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L45" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M45" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N45">
         <f t="shared" si="0"/>
         <v>1021.0985005999307</v>
+      </c>
+      <c r="O45" s="19">
+        <f t="shared" si="1"/>
+        <v>7.3856013262044939</v>
       </c>
       <c r="R45" s="9">
         <v>43026</v>
@@ -13835,20 +14025,24 @@
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L46" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M46" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N46">
         <f t="shared" si="0"/>
         <v>1021.2612205430163</v>
+      </c>
+      <c r="O46" s="19">
+        <f t="shared" si="1"/>
+        <v>8.3354546910875378</v>
       </c>
       <c r="R46" s="9">
         <v>43026</v>
@@ -14117,20 +14311,24 @@
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L47" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M47" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N47">
         <f t="shared" si="0"/>
         <v>1021.2612205430163</v>
+      </c>
+      <c r="O47" s="19">
+        <f t="shared" si="1"/>
+        <v>16.781029975290007</v>
       </c>
       <c r="R47" s="9">
         <v>43026</v>
@@ -14417,20 +14615,24 @@
       </c>
       <c r="J48" s="8"/>
       <c r="K48" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L48" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M48" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N48">
         <f t="shared" si="0"/>
         <v>1020.7320327829005</v>
+      </c>
+      <c r="O48" s="19">
+        <f t="shared" si="1"/>
+        <v>3.2049098769465449</v>
       </c>
       <c r="R48" s="9">
         <v>43026</v>
@@ -14699,20 +14901,24 @@
       </c>
       <c r="J49" s="8"/>
       <c r="K49" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.25217771670884</v>
       </c>
       <c r="L49" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76028272301154676</v>
       </c>
       <c r="M49" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2158637539999998E-3</v>
       </c>
       <c r="N49">
         <f t="shared" si="0"/>
         <v>1021.0861963783011</v>
+      </c>
+      <c r="O49" s="19">
+        <f t="shared" si="1"/>
+        <v>4.8689861892252857</v>
       </c>
       <c r="R49" s="9">
         <v>43026</v>
@@ -14983,20 +15189,24 @@
       </c>
       <c r="J50" s="8"/>
       <c r="K50" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L50" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M50" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N50">
         <f t="shared" si="0"/>
         <v>1021.4008023889601</v>
+      </c>
+      <c r="O50" s="19">
+        <f t="shared" si="1"/>
+        <v>3.6435901827223769</v>
       </c>
       <c r="R50" s="9">
         <v>43026</v>
@@ -15283,20 +15493,24 @@
         <v>42</v>
       </c>
       <c r="K51" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L51" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M51" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N51">
         <f t="shared" si="0"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O51" s="19">
+        <f t="shared" si="1"/>
+        <v>7.5632650417143443</v>
       </c>
       <c r="R51" s="9">
         <v>43026</v>
@@ -15565,20 +15779,24 @@
       </c>
       <c r="J52" s="8"/>
       <c r="K52" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.25217771670884</v>
       </c>
       <c r="L52" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76028272301154676</v>
       </c>
       <c r="M52" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2158637539999998E-3</v>
       </c>
       <c r="N52">
         <f t="shared" si="0"/>
         <v>1021.1617293120976</v>
+      </c>
+      <c r="O52" s="19">
+        <f t="shared" si="1"/>
+        <v>6.1997102257265082</v>
       </c>
       <c r="R52" s="9">
         <v>43026</v>
@@ -15849,20 +16067,24 @@
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L53" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M53" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N53">
         <f t="shared" si="0"/>
         <v>1021.4008023889601</v>
+      </c>
+      <c r="O53" s="19">
+        <f t="shared" si="1"/>
+        <v>1.6363563559666197</v>
       </c>
       <c r="R53" s="9">
         <v>43026</v>
@@ -16127,20 +16349,24 @@
       </c>
       <c r="J54" s="8"/>
       <c r="K54" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L54" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M54" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N54">
         <f t="shared" si="0"/>
         <v>1021.2612205430163</v>
+      </c>
+      <c r="O54" s="19">
+        <f t="shared" si="1"/>
+        <v>4.0474936367346057</v>
       </c>
       <c r="R54" s="9">
         <v>43026</v>
@@ -16427,20 +16653,24 @@
       </c>
       <c r="J55" s="8"/>
       <c r="K55" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L55" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M55" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N55">
         <f t="shared" si="0"/>
         <v>1021.0985005999307</v>
+      </c>
+      <c r="O55" s="19">
+        <f t="shared" si="1"/>
+        <v>8.7741932396801179</v>
       </c>
       <c r="R55" s="9">
         <v>43026</v>
@@ -16723,20 +16953,24 @@
       </c>
       <c r="J56" s="8"/>
       <c r="K56" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L56" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M56" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N56">
         <f t="shared" si="0"/>
         <v>1021.0229352475681</v>
+      </c>
+      <c r="O56" s="19">
+        <f t="shared" si="1"/>
+        <v>5.4437666106653468</v>
       </c>
       <c r="R56" s="9">
         <v>43026</v>
@@ -17019,20 +17253,24 @@
       </c>
       <c r="J57" s="8"/>
       <c r="K57" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L57" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M57" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N57">
         <f t="shared" si="0"/>
         <v>1020.7320327829005</v>
+      </c>
+      <c r="O57" s="19">
+        <f t="shared" si="1"/>
+        <v>7.8808891087634372</v>
       </c>
       <c r="R57" s="9">
         <v>43026</v>
@@ -17315,20 +17553,24 @@
       </c>
       <c r="J58" s="8"/>
       <c r="K58" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L58" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M58" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N58">
         <f t="shared" si="0"/>
         <v>1020.7320327829005</v>
+      </c>
+      <c r="O58" s="19">
+        <f t="shared" si="1"/>
+        <v>8.0942503129049381</v>
       </c>
       <c r="R58" s="9">
         <v>43026</v>
@@ -17615,20 +17857,24 @@
       </c>
       <c r="J59" s="8"/>
       <c r="K59" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L59" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76121220240660681</v>
       </c>
       <c r="M59" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2295732740000001E-3</v>
       </c>
       <c r="N59">
         <f t="shared" si="0"/>
         <v>1020.7320327829005</v>
+      </c>
+      <c r="O59" s="19">
+        <f t="shared" si="1"/>
+        <v>7.9909385719522117</v>
       </c>
       <c r="R59" s="9">
         <v>43026</v>
@@ -17911,20 +18157,24 @@
       </c>
       <c r="J60" s="8"/>
       <c r="K60" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L60" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M60" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N60">
         <f t="shared" si="0"/>
         <v>1020.9644870534015</v>
+      </c>
+      <c r="O60" s="19">
+        <f t="shared" si="1"/>
+        <v>8.5099118290056879</v>
       </c>
       <c r="R60" s="9">
         <v>43026</v>
@@ -18207,20 +18457,24 @@
       </c>
       <c r="J61" s="8"/>
       <c r="K61" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L61" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M61" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N61">
         <f t="shared" si="0"/>
         <v>1020.9644870534015</v>
+      </c>
+      <c r="O61" s="19">
+        <f t="shared" si="1"/>
+        <v>6.6947036036000398</v>
       </c>
       <c r="R61" s="9">
         <v>43026</v>
@@ -18503,20 +18757,24 @@
       </c>
       <c r="J62" s="8"/>
       <c r="K62" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L62" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76074425760000008</v>
       </c>
       <c r="M62" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N62">
         <f t="shared" si="0"/>
         <v>1021.4008023889601</v>
+      </c>
+      <c r="O62" s="19">
+        <f t="shared" si="1"/>
+        <v>7.2759416542087196</v>
       </c>
       <c r="R62" s="9">
         <v>43026</v>
@@ -18803,20 +19061,24 @@
       </c>
       <c r="J63" s="8"/>
       <c r="K63" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.35123703333397</v>
       </c>
       <c r="L63" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76089952447632669</v>
       </c>
       <c r="M63" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2248710660000004E-3</v>
       </c>
       <c r="N63">
         <f t="shared" si="0"/>
         <v>1021.3543787243402</v>
+      </c>
+      <c r="O63" s="19">
+        <f t="shared" si="1"/>
+        <v>3.9513067876176713</v>
       </c>
       <c r="R63" s="9">
         <v>43026</v>
@@ -19099,20 +19361,24 @@
       </c>
       <c r="J64" s="8"/>
       <c r="K64" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.35123703333397</v>
       </c>
       <c r="L64" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76089952447632669</v>
       </c>
       <c r="M64" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2248710660000004E-3</v>
       </c>
       <c r="N64">
         <f t="shared" si="0"/>
         <v>1021.3543787243402</v>
+      </c>
+      <c r="O64" s="19">
+        <f t="shared" si="1"/>
+        <v>5.4189992405837346</v>
       </c>
       <c r="R64" s="9">
         <v>43026</v>
@@ -19395,20 +19661,24 @@
       </c>
       <c r="J65" s="8"/>
       <c r="K65" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L65" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M65" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N65">
         <f t="shared" si="0"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O65" s="19">
+        <f t="shared" si="1"/>
+        <v>2.9907028432922731</v>
       </c>
       <c r="R65" s="9">
         <v>43026</v>
@@ -19693,20 +19963,24 @@
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.27708768547382</v>
       </c>
       <c r="L66" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.760435858711068</v>
       </c>
       <c r="M66" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N66">
         <f t="shared" si="0"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O66" s="19">
+        <f t="shared" si="1"/>
+        <v>6.9071529228252802</v>
       </c>
       <c r="R66" s="9">
         <v>43026</v>
@@ -19993,20 +20267,24 @@
       </c>
       <c r="J67" s="8"/>
       <c r="K67" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>997.35123703333397</v>
       </c>
       <c r="L67" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76089952447632669</v>
       </c>
       <c r="M67" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.2248710660000004E-3</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N130" si="4" xml:space="preserve"> K67 + (L67*G67) + M67*G67^(3/2) + 0.00048314*G67^2</f>
+        <f t="shared" ref="N67:N130" si="5" xml:space="preserve"> K67 + (L67*G67) + M67*G67^(3/2) + 0.00048314*G67^2</f>
         <v>1021.2787876796716</v>
+      </c>
+      <c r="O67" s="19">
+        <f t="shared" ref="O67:O130" si="6">I67*(1/     (1-   (0.001*N67/1.84)))</f>
+        <v>6.562429211737423</v>
       </c>
       <c r="R67" s="9">
         <v>43026</v>
@@ -20289,20 +20567,24 @@
       </c>
       <c r="J68" s="8"/>
       <c r="K68" s="12">
-        <f t="shared" ref="K68:K131" si="5">1000*(1-(F68+288.9414)/(508929.2*(F68+68.12963))*(F68-3.9863)^2)</f>
+        <f t="shared" ref="K68:K131" si="7">1000*(1-(F68+288.9414)/(508929.2*(F68+68.12963))*(F68-3.9863)^2)</f>
         <v>997.32661753089724</v>
       </c>
       <c r="L68" s="15">
-        <f t="shared" ref="L68:L131" si="6" xml:space="preserve"> 0.824493 - 0.0040899*F68 + 0.000076438*F68^2 -0.00000082467*F68^3 + 0.0000000053675*F68^4</f>
+        <f t="shared" ref="L68:L131" si="8" xml:space="preserve"> 0.824493 - 0.0040899*F68 + 0.000076438*F68^2 -0.00000082467*F68^3 + 0.0000000053675*F68^4</f>
         <v>0.76074425760000008</v>
       </c>
       <c r="M68" s="17">
-        <f t="shared" ref="M68:M131" si="7" xml:space="preserve"> -0.005724 + 0.00010227*F68 - 0.0000016546*F68^2</f>
+        <f t="shared" ref="M68:M131" si="9" xml:space="preserve"> -0.005724 + 0.00010227*F68 - 0.0000016546*F68^2</f>
         <v>-4.2225696E-3</v>
       </c>
       <c r="N68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1021.3252208670636</v>
+      </c>
+      <c r="O68" s="19">
+        <f t="shared" si="6"/>
+        <v>9.8486971939448846</v>
       </c>
       <c r="R68" s="9">
         <v>43026</v>
@@ -20585,20 +20867,24 @@
       </c>
       <c r="J69" s="8"/>
       <c r="K69" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L69" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M69" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N69">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L69" s="15">
+        <v>1021.0985005999307</v>
+      </c>
+      <c r="O69" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M69" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N69">
-        <f t="shared" si="4"/>
-        <v>1021.0985005999307</v>
+        <v>3.4827143460958219</v>
       </c>
       <c r="R69" s="9">
         <v>43026</v>
@@ -20881,20 +21167,24 @@
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L70" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M70" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N70">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L70" s="15">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O70" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M70" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N70">
-        <f t="shared" si="4"/>
-        <v>1021.2612205430163</v>
+        <v>1.8810395191265215</v>
       </c>
       <c r="R70" s="9">
         <v>43026</v>
@@ -21179,20 +21469,24 @@
       </c>
       <c r="J71" s="8"/>
       <c r="K71" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L71" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M71" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N71">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L71" s="15">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O71" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M71" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N71">
-        <f t="shared" si="4"/>
-        <v>1021.2612205430163</v>
+        <v>9.4007028775462835</v>
       </c>
       <c r="R71" s="9">
         <v>43026</v>
@@ -21479,20 +21773,24 @@
       </c>
       <c r="J72" s="8"/>
       <c r="K72" s="12">
+        <f t="shared" si="7"/>
+        <v>997.25217771670884</v>
+      </c>
+      <c r="L72" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M72" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N72">
         <f t="shared" si="5"/>
-        <v>997.25217771670884</v>
-      </c>
-      <c r="L72" s="15">
+        <v>1021.0861963783011</v>
+      </c>
+      <c r="O72" s="19">
         <f t="shared" si="6"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M72" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N72">
-        <f t="shared" si="4"/>
-        <v>1021.0861963783011</v>
+        <v>6.2687916326435387</v>
       </c>
       <c r="R72" s="9">
         <v>43026</v>
@@ -21777,20 +22075,24 @@
       </c>
       <c r="J73" s="8"/>
       <c r="K73" s="12">
+        <f t="shared" si="7"/>
+        <v>997.25217771670884</v>
+      </c>
+      <c r="L73" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M73" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N73">
         <f t="shared" si="5"/>
-        <v>997.25217771670884</v>
-      </c>
-      <c r="L73" s="15">
+        <v>1021.0861963783011</v>
+      </c>
+      <c r="O73" s="19">
         <f t="shared" si="6"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M73" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N73">
-        <f t="shared" si="4"/>
-        <v>1021.0861963783011</v>
+        <v>5.8531190691886801</v>
       </c>
       <c r="R73" s="9">
         <v>43026</v>
@@ -22077,20 +22379,24 @@
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L74" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M74" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N74">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L74" s="15">
+        <v>1020.7320327829005</v>
+      </c>
+      <c r="O74" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M74" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N74">
-        <f t="shared" si="4"/>
-        <v>1020.7320327829005</v>
+        <v>1.9584312632777765</v>
       </c>
       <c r="R74" s="9">
         <v>43026</v>
@@ -22377,20 +22683,24 @@
         <v>42</v>
       </c>
       <c r="K75" s="12">
+        <f t="shared" si="7"/>
+        <v>997.27708768547382</v>
+      </c>
+      <c r="L75" s="15">
+        <f t="shared" si="8"/>
+        <v>0.760435858711068</v>
+      </c>
+      <c r="M75" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2180659439999997E-3</v>
+      </c>
+      <c r="N75">
         <f t="shared" si="5"/>
-        <v>997.27708768547382</v>
-      </c>
-      <c r="L75" s="15">
+        <v>1021.1155677024707</v>
+      </c>
+      <c r="O75" s="19">
         <f t="shared" si="6"/>
-        <v>0.760435858711068</v>
-      </c>
-      <c r="M75" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2180659439999997E-3</v>
-      </c>
-      <c r="N75">
-        <f t="shared" si="4"/>
-        <v>1021.1155677024707</v>
+        <v>5.936466500359268</v>
       </c>
       <c r="R75" s="9">
         <v>43026</v>
@@ -22675,20 +22985,24 @@
       </c>
       <c r="J76" s="8"/>
       <c r="K76" s="12">
+        <f t="shared" si="7"/>
+        <v>997.25217771670884</v>
+      </c>
+      <c r="L76" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M76" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N76">
         <f t="shared" si="5"/>
-        <v>997.25217771670884</v>
-      </c>
-      <c r="L76" s="15">
+        <v>1021.1617293120976</v>
+      </c>
+      <c r="O76" s="19">
         <f t="shared" si="6"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M76" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N76">
-        <f t="shared" si="4"/>
-        <v>1021.1617293120976</v>
+        <v>5.3772767561303132</v>
       </c>
       <c r="R76" s="9">
         <v>43026</v>
@@ -22973,20 +23287,24 @@
         <v>62</v>
       </c>
       <c r="K77" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L77" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M77" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N77">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L77" s="15">
+        <v>1021.4008023889601</v>
+      </c>
+      <c r="O77" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M77" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N77">
-        <f t="shared" si="4"/>
-        <v>1021.4008023889601</v>
+        <v>2.5466919660854122</v>
       </c>
       <c r="R77" s="9">
         <v>43026</v>
@@ -23273,20 +23591,24 @@
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="12">
+        <f t="shared" si="7"/>
+        <v>997.35123703333397</v>
+      </c>
+      <c r="L78" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76089952447632669</v>
+      </c>
+      <c r="M78" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2248710660000004E-3</v>
+      </c>
+      <c r="N78">
         <f t="shared" si="5"/>
-        <v>997.35123703333397</v>
-      </c>
-      <c r="L78" s="15">
+        <v>1021.2787876796716</v>
+      </c>
+      <c r="O78" s="19">
         <f t="shared" si="6"/>
-        <v>0.76089952447632669</v>
-      </c>
-      <c r="M78" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2248710660000004E-3</v>
-      </c>
-      <c r="N78">
-        <f t="shared" si="4"/>
-        <v>1021.2787876796716</v>
+        <v>3.2092975734113152</v>
       </c>
       <c r="R78" s="9">
         <v>43026</v>
@@ -23573,20 +23895,24 @@
       </c>
       <c r="J79" s="8"/>
       <c r="K79" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L79" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M79" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N79">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L79" s="15">
+        <v>1021.0229352475681</v>
+      </c>
+      <c r="O79" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M79" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N79">
-        <f t="shared" si="4"/>
-        <v>1021.0229352475681</v>
+        <v>8.0319709587819297</v>
       </c>
       <c r="R79" s="9">
         <v>43026</v>
@@ -23871,20 +24197,24 @@
       </c>
       <c r="J80" s="8"/>
       <c r="K80" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L80" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M80" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N80">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L80" s="15">
+        <v>1021.0229352475681</v>
+      </c>
+      <c r="O80" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M80" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N80">
-        <f t="shared" si="4"/>
-        <v>1021.0229352475681</v>
+        <v>5.8706405916915188</v>
       </c>
       <c r="R80" s="9">
         <v>43026</v>
@@ -24169,20 +24499,24 @@
       </c>
       <c r="J81" s="8"/>
       <c r="K81" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L81" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M81" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N81">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L81" s="15">
+        <v>1020.7320327829005</v>
+      </c>
+      <c r="O81" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M81" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N81">
-        <f t="shared" si="4"/>
-        <v>1020.7320327829005</v>
+        <v>7.4204780893001985</v>
       </c>
       <c r="R81" s="9">
         <v>43026</v>
@@ -24467,20 +24801,24 @@
       </c>
       <c r="J82" s="8"/>
       <c r="K82" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L82" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M82" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N82">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L82" s="15">
+        <v>1020.7320327829005</v>
+      </c>
+      <c r="O82" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M82" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N82">
-        <f t="shared" si="4"/>
-        <v>1020.7320327829005</v>
+        <v>7.4339535337722937</v>
       </c>
       <c r="R82" s="9">
         <v>43026</v>
@@ -24765,20 +25103,24 @@
       </c>
       <c r="J83" s="8"/>
       <c r="K83" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L83" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M83" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N83">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L83" s="15">
+        <v>1020.7320327829005</v>
+      </c>
+      <c r="O83" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M83" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N83">
-        <f t="shared" si="4"/>
-        <v>1020.7320327829005</v>
+        <v>9.7023200199082513</v>
       </c>
       <c r="R83" s="9">
         <v>43026</v>
@@ -25065,20 +25407,24 @@
       </c>
       <c r="J84" s="8"/>
       <c r="K84" s="12">
+        <f t="shared" si="7"/>
+        <v>997.27708768547382</v>
+      </c>
+      <c r="L84" s="15">
+        <f t="shared" si="8"/>
+        <v>0.760435858711068</v>
+      </c>
+      <c r="M84" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2180659439999997E-3</v>
+      </c>
+      <c r="N84">
         <f t="shared" si="5"/>
-        <v>997.27708768547382</v>
-      </c>
-      <c r="L84" s="15">
+        <v>1020.9644870534015</v>
+      </c>
+      <c r="O84" s="19">
         <f t="shared" si="6"/>
-        <v>0.760435858711068</v>
-      </c>
-      <c r="M84" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2180659439999997E-3</v>
-      </c>
-      <c r="N84">
-        <f t="shared" si="4"/>
-        <v>1020.9644870534015</v>
+        <v>6.7755792176032621</v>
       </c>
       <c r="R84" s="9">
         <v>43026</v>
@@ -25363,20 +25709,24 @@
       </c>
       <c r="J85" s="8"/>
       <c r="K85" s="12">
+        <f t="shared" si="7"/>
+        <v>997.27708768547382</v>
+      </c>
+      <c r="L85" s="15">
+        <f t="shared" si="8"/>
+        <v>0.760435858711068</v>
+      </c>
+      <c r="M85" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2180659439999997E-3</v>
+      </c>
+      <c r="N85">
         <f t="shared" si="5"/>
-        <v>997.27708768547382</v>
-      </c>
-      <c r="L85" s="15">
+        <v>1020.9644870534015</v>
+      </c>
+      <c r="O85" s="19">
         <f t="shared" si="6"/>
-        <v>0.760435858711068</v>
-      </c>
-      <c r="M85" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2180659439999997E-3</v>
-      </c>
-      <c r="N85">
-        <f t="shared" si="4"/>
-        <v>1020.9644870534015</v>
+        <v>5.9443576292368139</v>
       </c>
       <c r="R85" s="9">
         <v>43026</v>
@@ -25661,20 +26011,24 @@
       </c>
       <c r="J86" s="8"/>
       <c r="K86" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L86" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M86" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N86">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L86" s="15">
+        <v>1021.4008023889601</v>
+      </c>
+      <c r="O86" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M86" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N86">
-        <f t="shared" si="4"/>
-        <v>1021.4008023889601</v>
+        <v>8.9212889791641654</v>
       </c>
       <c r="R86" s="9">
         <v>43026</v>
@@ -25961,20 +26315,24 @@
       </c>
       <c r="J87" s="8"/>
       <c r="K87" s="12">
+        <f t="shared" si="7"/>
+        <v>997.35123703333397</v>
+      </c>
+      <c r="L87" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76089952447632669</v>
+      </c>
+      <c r="M87" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2248710660000004E-3</v>
+      </c>
+      <c r="N87">
         <f t="shared" si="5"/>
-        <v>997.35123703333397</v>
-      </c>
-      <c r="L87" s="15">
+        <v>1021.3543787243402</v>
+      </c>
+      <c r="O87" s="19">
         <f t="shared" si="6"/>
-        <v>0.76089952447632669</v>
-      </c>
-      <c r="M87" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2248710660000004E-3</v>
-      </c>
-      <c r="N87">
-        <f t="shared" si="4"/>
-        <v>1021.3543787243402</v>
+        <v>6.2663500135825183</v>
       </c>
       <c r="R87" s="9">
         <v>43026</v>
@@ -26261,20 +26619,24 @@
       </c>
       <c r="J88" s="8"/>
       <c r="K88" s="12">
+        <f t="shared" si="7"/>
+        <v>997.27708768547382</v>
+      </c>
+      <c r="L88" s="15">
+        <f t="shared" si="8"/>
+        <v>0.760435858711068</v>
+      </c>
+      <c r="M88" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2180659439999997E-3</v>
+      </c>
+      <c r="N88">
         <f t="shared" si="5"/>
-        <v>997.27708768547382</v>
-      </c>
-      <c r="L88" s="15">
+        <v>1021.1155677024707</v>
+      </c>
+      <c r="O88" s="19">
         <f t="shared" si="6"/>
-        <v>0.760435858711068</v>
-      </c>
-      <c r="M88" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2180659439999997E-3</v>
-      </c>
-      <c r="N88">
-        <f t="shared" si="4"/>
-        <v>1021.1155677024707</v>
+        <v>8.6305707145647048</v>
       </c>
       <c r="R88" s="9">
         <v>43026</v>
@@ -26559,20 +26921,24 @@
       </c>
       <c r="J89" s="8"/>
       <c r="K89" s="12">
+        <f t="shared" si="7"/>
+        <v>997.27708768547382</v>
+      </c>
+      <c r="L89" s="15">
+        <f t="shared" si="8"/>
+        <v>0.760435858711068</v>
+      </c>
+      <c r="M89" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2180659439999997E-3</v>
+      </c>
+      <c r="N89">
         <f t="shared" si="5"/>
-        <v>997.27708768547382</v>
-      </c>
-      <c r="L89" s="15">
+        <v>1021.1155677024707</v>
+      </c>
+      <c r="O89" s="19">
         <f t="shared" si="6"/>
-        <v>0.760435858711068</v>
-      </c>
-      <c r="M89" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2180659439999997E-3</v>
-      </c>
-      <c r="N89">
-        <f t="shared" si="4"/>
-        <v>1021.1155677024707</v>
+        <v>6.817274550374723</v>
       </c>
       <c r="R89" s="9">
         <v>43026</v>
@@ -26857,20 +27223,24 @@
       </c>
       <c r="J90" s="8"/>
       <c r="K90" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L90" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M90" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N90">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L90" s="15">
+        <v>1021.3252208670636</v>
+      </c>
+      <c r="O90" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M90" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N90">
-        <f t="shared" si="4"/>
-        <v>1021.3252208670636</v>
+        <v>7.4101220101406406</v>
       </c>
       <c r="R90" s="9">
         <v>43026</v>
@@ -27155,20 +27525,24 @@
       </c>
       <c r="J91" s="3"/>
       <c r="K91" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L91" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M91" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N91">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L91" s="15">
+        <v>1021.0985005999307</v>
+      </c>
+      <c r="O91" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M91" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N91">
-        <f t="shared" si="4"/>
-        <v>1021.0985005999307</v>
+        <v>7.6282678741905254</v>
       </c>
       <c r="R91" s="9">
         <v>43026</v>
@@ -27453,20 +27827,24 @@
       </c>
       <c r="J92" s="3"/>
       <c r="K92" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L92" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M92" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N92">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L92" s="15">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O92" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M92" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N92">
-        <f t="shared" si="4"/>
-        <v>1021.2612205430163</v>
+        <v>7.4185322014774764</v>
       </c>
       <c r="R92" s="9">
         <v>43026</v>
@@ -27751,20 +28129,24 @@
       </c>
       <c r="J93" s="3"/>
       <c r="K93" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L93" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M93" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N93">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L93" s="15">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O93" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M93" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N93">
-        <f t="shared" si="4"/>
-        <v>1021.2612205430163</v>
+        <v>9.6861174760278459</v>
       </c>
       <c r="R93" s="9">
         <v>43026</v>
@@ -28051,20 +28433,24 @@
       </c>
       <c r="J94" s="3"/>
       <c r="K94" s="12">
+        <f t="shared" si="7"/>
+        <v>997.25217771670884</v>
+      </c>
+      <c r="L94" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M94" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N94">
         <f t="shared" si="5"/>
-        <v>997.25217771670884</v>
-      </c>
-      <c r="L94" s="15">
+        <v>1021.0861963783011</v>
+      </c>
+      <c r="O94" s="19">
         <f t="shared" si="6"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M94" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N94">
-        <f t="shared" si="4"/>
-        <v>1021.0861963783011</v>
+        <v>6.264297875200783</v>
       </c>
       <c r="R94" s="9">
         <v>43026</v>
@@ -28349,20 +28735,24 @@
       </c>
       <c r="J95" s="3"/>
       <c r="K95" s="12">
+        <f t="shared" si="7"/>
+        <v>997.25217771670884</v>
+      </c>
+      <c r="L95" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M95" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N95">
         <f t="shared" si="5"/>
-        <v>997.25217771670884</v>
-      </c>
-      <c r="L95" s="15">
+        <v>1021.0861963783011</v>
+      </c>
+      <c r="O95" s="19">
         <f t="shared" si="6"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M95" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N95">
-        <f t="shared" si="4"/>
-        <v>1021.0861963783011</v>
+        <v>6.3272104793993567</v>
       </c>
       <c r="R95" s="9">
         <v>43026</v>
@@ -28647,20 +29037,24 @@
       </c>
       <c r="J96" s="3"/>
       <c r="K96" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L96" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M96" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N96">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L96" s="15">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O96" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M96" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N96">
-        <f t="shared" si="4"/>
-        <v>1021.2612205430163</v>
+        <v>5.1846573125745339</v>
       </c>
       <c r="R96" s="9">
         <v>43026</v>
@@ -28945,20 +29339,24 @@
       </c>
       <c r="J97" s="3"/>
       <c r="K97" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L97" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M97" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N97">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L97" s="15">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O97" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M97" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N97">
-        <f t="shared" si="4"/>
-        <v>1021.2612205430163</v>
+        <v>6.9488341614566362</v>
       </c>
       <c r="R97" s="9">
         <v>43026</v>
@@ -29237,20 +29635,24 @@
       </c>
       <c r="J98" s="3"/>
       <c r="K98" s="12">
+        <f t="shared" si="7"/>
+        <v>997.35123703333397</v>
+      </c>
+      <c r="L98" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76089952447632669</v>
+      </c>
+      <c r="M98" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2248710660000004E-3</v>
+      </c>
+      <c r="N98">
         <f t="shared" si="5"/>
-        <v>997.35123703333397</v>
-      </c>
-      <c r="L98" s="15">
+        <v>1021.2787876796716</v>
+      </c>
+      <c r="O98" s="19">
         <f t="shared" si="6"/>
-        <v>0.76089952447632669</v>
-      </c>
-      <c r="M98" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2248710660000004E-3</v>
-      </c>
-      <c r="N98">
-        <f t="shared" si="4"/>
-        <v>1021.2787876796716</v>
+        <v>3.5104501468266629</v>
       </c>
       <c r="R98" s="9">
         <v>43026</v>
@@ -29527,20 +29929,24 @@
       </c>
       <c r="J99" s="3"/>
       <c r="K99" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L99" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M99" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N99">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L99" s="15">
+        <v>1021.0229352475681</v>
+      </c>
+      <c r="O99" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M99" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N99">
-        <f t="shared" si="4"/>
-        <v>1021.0229352475681</v>
+        <v>5.3516516989702252</v>
       </c>
       <c r="R99" s="9">
         <v>43026</v>
@@ -29827,20 +30233,24 @@
       </c>
       <c r="J100" s="3"/>
       <c r="K100" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L100" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M100" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N100">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L100" s="15">
+        <v>1021.0229352475681</v>
+      </c>
+      <c r="O100" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M100" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N100">
-        <f t="shared" si="4"/>
-        <v>1021.0229352475681</v>
+        <v>1.2581548914455611</v>
       </c>
       <c r="R100" s="9">
         <v>43026</v>
@@ -30123,20 +30533,24 @@
       </c>
       <c r="J101" s="3"/>
       <c r="K101" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L101" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M101" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N101">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L101" s="15">
+        <v>1020.7320327829005</v>
+      </c>
+      <c r="O101" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M101" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N101">
-        <f t="shared" si="4"/>
-        <v>1020.7320327829005</v>
+        <v>6.755689495343522</v>
       </c>
       <c r="R101" s="9">
         <v>43026</v>
@@ -30419,20 +30833,24 @@
       </c>
       <c r="J102" s="3"/>
       <c r="K102" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L102" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M102" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N102">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L102" s="15">
+        <v>1020.7320327829005</v>
+      </c>
+      <c r="O102" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M102" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N102">
-        <f t="shared" si="4"/>
-        <v>1020.7320327829005</v>
+        <v>4.3233717681304125</v>
       </c>
       <c r="R102" s="9">
         <v>43026</v>
@@ -30715,20 +31133,24 @@
       </c>
       <c r="J103" s="3"/>
       <c r="K103" s="12">
+        <f t="shared" si="7"/>
+        <v>997.27708768547382</v>
+      </c>
+      <c r="L103" s="15">
+        <f t="shared" si="8"/>
+        <v>0.760435858711068</v>
+      </c>
+      <c r="M103" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2180659439999997E-3</v>
+      </c>
+      <c r="N103">
         <f t="shared" si="5"/>
-        <v>997.27708768547382</v>
-      </c>
-      <c r="L103" s="15">
+        <v>1020.9644870534015</v>
+      </c>
+      <c r="O103" s="19">
         <f t="shared" si="6"/>
-        <v>0.760435858711068</v>
-      </c>
-      <c r="M103" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2180659439999997E-3</v>
-      </c>
-      <c r="N103">
-        <f t="shared" si="4"/>
-        <v>1020.9644870534015</v>
+        <v>8.3593933251663586</v>
       </c>
       <c r="R103" s="9">
         <v>43026</v>
@@ -31011,20 +31433,24 @@
       </c>
       <c r="J104" s="3"/>
       <c r="K104" s="12">
+        <f t="shared" si="7"/>
+        <v>997.25217771670884</v>
+      </c>
+      <c r="L104" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M104" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N104">
         <f t="shared" si="5"/>
-        <v>997.25217771670884</v>
-      </c>
-      <c r="L104" s="15">
+        <v>1021.1617293120976</v>
+      </c>
+      <c r="O104" s="19">
         <f t="shared" si="6"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M104" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N104">
-        <f t="shared" si="4"/>
-        <v>1021.1617293120976</v>
+        <v>3.8065636543605312</v>
       </c>
       <c r="R104" s="9">
         <v>43026</v>
@@ -31307,20 +31733,24 @@
       </c>
       <c r="J105" s="3"/>
       <c r="K105" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L105" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M105" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N105">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L105" s="15">
+        <v>1021.4008023889601</v>
+      </c>
+      <c r="O105" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M105" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N105">
-        <f t="shared" si="4"/>
-        <v>1021.4008023889601</v>
+        <v>8.2447185627548922</v>
       </c>
       <c r="R105" s="9">
         <v>43026</v>
@@ -31607,20 +32037,24 @@
       </c>
       <c r="J106" s="3"/>
       <c r="K106" s="12">
+        <f t="shared" si="7"/>
+        <v>997.35123703333397</v>
+      </c>
+      <c r="L106" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76089952447632669</v>
+      </c>
+      <c r="M106" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2248710660000004E-3</v>
+      </c>
+      <c r="N106">
         <f t="shared" si="5"/>
-        <v>997.35123703333397</v>
-      </c>
-      <c r="L106" s="15">
+        <v>1021.3543787243402</v>
+      </c>
+      <c r="O106" s="19">
         <f t="shared" si="6"/>
-        <v>0.76089952447632669</v>
-      </c>
-      <c r="M106" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2248710660000004E-3</v>
-      </c>
-      <c r="N106">
-        <f t="shared" si="4"/>
-        <v>1021.3543787243402</v>
+        <v>6.4663877292241407</v>
       </c>
       <c r="R106" s="9">
         <v>43026</v>
@@ -31903,20 +32337,24 @@
       </c>
       <c r="J107" s="3"/>
       <c r="K107" s="12">
+        <f t="shared" si="7"/>
+        <v>997.35123703333397</v>
+      </c>
+      <c r="L107" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76089952447632669</v>
+      </c>
+      <c r="M107" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2248710660000004E-3</v>
+      </c>
+      <c r="N107">
         <f t="shared" si="5"/>
-        <v>997.35123703333397</v>
-      </c>
-      <c r="L107" s="15">
+        <v>1021.3543787243402</v>
+      </c>
+      <c r="O107" s="19">
         <f t="shared" si="6"/>
-        <v>0.76089952447632669</v>
-      </c>
-      <c r="M107" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2248710660000004E-3</v>
-      </c>
-      <c r="N107">
-        <f t="shared" si="4"/>
-        <v>1021.3543787243402</v>
+        <v>4.3378965302059758</v>
       </c>
       <c r="R107" s="9">
         <v>43026</v>
@@ -32199,20 +32637,24 @@
       </c>
       <c r="J108" s="3"/>
       <c r="K108" s="12">
+        <f t="shared" si="7"/>
+        <v>997.27708768547382</v>
+      </c>
+      <c r="L108" s="15">
+        <f t="shared" si="8"/>
+        <v>0.760435858711068</v>
+      </c>
+      <c r="M108" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2180659439999997E-3</v>
+      </c>
+      <c r="N108">
         <f t="shared" si="5"/>
-        <v>997.27708768547382</v>
-      </c>
-      <c r="L108" s="15">
+        <v>1021.1155677024707</v>
+      </c>
+      <c r="O108" s="19">
         <f t="shared" si="6"/>
-        <v>0.760435858711068</v>
-      </c>
-      <c r="M108" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2180659439999997E-3</v>
-      </c>
-      <c r="N108">
-        <f t="shared" si="4"/>
-        <v>1021.1155677024707</v>
+        <v>5.8106367789284885</v>
       </c>
       <c r="R108" s="9">
         <v>43026</v>
@@ -32495,20 +32937,24 @@
       </c>
       <c r="J109" s="3"/>
       <c r="K109" s="12">
+        <f t="shared" si="7"/>
+        <v>997.35123703333397</v>
+      </c>
+      <c r="L109" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76089952447632669</v>
+      </c>
+      <c r="M109" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2248710660000004E-3</v>
+      </c>
+      <c r="N109">
         <f t="shared" si="5"/>
-        <v>997.35123703333397</v>
-      </c>
-      <c r="L109" s="15">
+        <v>1021.2787876796716</v>
+      </c>
+      <c r="O109" s="19">
         <f t="shared" si="6"/>
-        <v>0.76089952447632669</v>
-      </c>
-      <c r="M109" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2248710660000004E-3</v>
-      </c>
-      <c r="N109">
-        <f t="shared" si="4"/>
-        <v>1021.2787876796716</v>
+        <v>6.7467166074095006</v>
       </c>
       <c r="R109" s="9">
         <v>43026</v>
@@ -32797,20 +33243,24 @@
       </c>
       <c r="J110" s="3"/>
       <c r="K110" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L110" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M110" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N110">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L110" s="15">
+        <v>1020.7320327829005</v>
+      </c>
+      <c r="O110" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M110" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N110">
-        <f t="shared" si="4"/>
-        <v>1020.7320327829005</v>
+        <v>1.3116099286172263</v>
       </c>
       <c r="R110" s="9">
         <v>43026</v>
@@ -33093,20 +33543,24 @@
       </c>
       <c r="J111" s="3"/>
       <c r="K111" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L111" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M111" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N111">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L111" s="15">
+        <v>1021.3252208670636</v>
+      </c>
+      <c r="O111" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M111" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N111">
-        <f t="shared" si="4"/>
-        <v>1021.3252208670636</v>
+        <v>6.2414039496998965</v>
       </c>
       <c r="R111" s="9">
         <v>43026</v>
@@ -33391,20 +33845,24 @@
       </c>
       <c r="J112" s="3"/>
       <c r="K112" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L112" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M112" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N112">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L112" s="15">
+        <v>1021.0985005999307</v>
+      </c>
+      <c r="O112" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M112" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N112">
-        <f t="shared" si="4"/>
-        <v>1021.0985005999307</v>
+        <v>4.9926395335644616</v>
       </c>
       <c r="R112" s="9">
         <v>43026</v>
@@ -33691,20 +34149,24 @@
       </c>
       <c r="J113" s="3"/>
       <c r="K113" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L113" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M113" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N113">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L113" s="15">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O113" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M113" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N113">
-        <f t="shared" si="4"/>
-        <v>1021.2612205430163</v>
+        <v>7.1263755258664272</v>
       </c>
       <c r="R113" s="9">
         <v>43026</v>
@@ -33991,20 +34453,24 @@
       </c>
       <c r="J114" s="3"/>
       <c r="K114" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L114" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M114" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N114">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L114" s="15">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O114" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M114" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N114">
-        <f t="shared" si="4"/>
-        <v>1021.2612205430163</v>
+        <v>13.699900727115025</v>
       </c>
       <c r="R114" s="9">
         <v>43026</v>
@@ -34285,20 +34751,24 @@
       </c>
       <c r="J115" s="3"/>
       <c r="K115" s="12">
+        <f t="shared" si="7"/>
+        <v>997.25217771670884</v>
+      </c>
+      <c r="L115" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M115" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N115">
         <f t="shared" si="5"/>
-        <v>997.25217771670884</v>
-      </c>
-      <c r="L115" s="15">
+        <v>1021.0861963783011</v>
+      </c>
+      <c r="O115" s="19">
         <f t="shared" si="6"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M115" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N115">
-        <f t="shared" si="4"/>
-        <v>1021.0861963783011</v>
+        <v>5.1992773612677956</v>
       </c>
       <c r="R115" s="9">
         <v>43026</v>
@@ -34583,20 +35053,24 @@
       </c>
       <c r="J116" s="3"/>
       <c r="K116" s="12">
+        <f t="shared" si="7"/>
+        <v>997.25217771670884</v>
+      </c>
+      <c r="L116" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M116" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N116">
         <f t="shared" si="5"/>
-        <v>997.25217771670884</v>
-      </c>
-      <c r="L116" s="15">
+        <v>1021.0861963783011</v>
+      </c>
+      <c r="O116" s="19">
         <f t="shared" si="6"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M116" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N116">
-        <f t="shared" si="4"/>
-        <v>1021.0861963783011</v>
+        <v>5.7003313161350029</v>
       </c>
       <c r="R116" s="9">
         <v>43026</v>
@@ -34881,20 +35355,24 @@
       </c>
       <c r="J117" s="3"/>
       <c r="K117" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L117" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M117" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N117">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L117" s="15">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O117" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M117" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N117">
-        <f t="shared" si="4"/>
-        <v>1021.2612205430163</v>
+        <v>7.488200331815495</v>
       </c>
       <c r="R117" s="9">
         <v>43026</v>
@@ -35179,20 +35657,24 @@
       </c>
       <c r="J118" s="3"/>
       <c r="K118" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L118" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M118" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N118">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L118" s="15">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O118" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M118" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N118">
-        <f t="shared" si="4"/>
-        <v>1021.2612205430163</v>
+        <v>7.9354247814047172</v>
       </c>
       <c r="R118" s="9">
         <v>43026</v>
@@ -35479,20 +35961,24 @@
       </c>
       <c r="J119" s="3"/>
       <c r="K119" s="12">
+        <f t="shared" si="7"/>
+        <v>997.25217771670884</v>
+      </c>
+      <c r="L119" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M119" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N119">
         <f t="shared" si="5"/>
-        <v>997.25217771670884</v>
-      </c>
-      <c r="L119" s="15">
+        <v>1021.1617293120976</v>
+      </c>
+      <c r="O119" s="19">
         <f t="shared" si="6"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M119" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N119">
-        <f t="shared" si="4"/>
-        <v>1021.1617293120976</v>
+        <v>3.417817779387466</v>
       </c>
       <c r="R119" s="9">
         <v>43026</v>
@@ -35775,20 +36261,24 @@
       </c>
       <c r="J120" s="3"/>
       <c r="K120" s="12">
+        <f t="shared" si="7"/>
+        <v>997.25217771670884</v>
+      </c>
+      <c r="L120" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M120" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N120">
         <f t="shared" si="5"/>
-        <v>997.25217771670884</v>
-      </c>
-      <c r="L120" s="15">
+        <v>1021.1617293120976</v>
+      </c>
+      <c r="O120" s="19">
         <f t="shared" si="6"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M120" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N120">
-        <f t="shared" si="4"/>
-        <v>1021.1617293120976</v>
+        <v>3.5863492280752114</v>
       </c>
       <c r="R120" s="9">
         <v>43026</v>
@@ -36037,20 +36527,24 @@
       </c>
       <c r="J121" s="3"/>
       <c r="K121" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L121" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M121" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N121">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L121" s="15">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O121" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M121" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N121">
-        <f t="shared" si="4"/>
-        <v>1021.2612205430163</v>
+        <v>6.0453958261055467</v>
       </c>
       <c r="R121" s="9">
         <v>43026</v>
@@ -36335,20 +36829,24 @@
       </c>
       <c r="J122" s="3"/>
       <c r="K122" s="12">
+        <f t="shared" si="7"/>
+        <v>997.35123703333397</v>
+      </c>
+      <c r="L122" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76089952447632669</v>
+      </c>
+      <c r="M122" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2248710660000004E-3</v>
+      </c>
+      <c r="N122">
         <f t="shared" si="5"/>
-        <v>997.35123703333397</v>
-      </c>
-      <c r="L122" s="15">
+        <v>1021.2787876796716</v>
+      </c>
+      <c r="O122" s="19">
         <f t="shared" si="6"/>
-        <v>0.76089952447632669</v>
-      </c>
-      <c r="M122" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2248710660000004E-3</v>
-      </c>
-      <c r="N122">
-        <f t="shared" si="4"/>
-        <v>1021.2787876796716</v>
+        <v>3.8228397565634786</v>
       </c>
       <c r="R122" s="9">
         <v>43026</v>
@@ -36597,20 +37095,24 @@
       </c>
       <c r="J123" s="3"/>
       <c r="K123" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L123" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M123" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N123">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L123" s="15">
+        <v>1021.0229352475681</v>
+      </c>
+      <c r="O123" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M123" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N123">
-        <f t="shared" si="4"/>
-        <v>1021.0229352475681</v>
+        <v>5.996456080836075</v>
       </c>
       <c r="R123" s="9">
         <v>43026</v>
@@ -36897,20 +37399,24 @@
       </c>
       <c r="J124" s="3"/>
       <c r="K124" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L124" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M124" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N124">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L124" s="15">
+        <v>1021.0229352475681</v>
+      </c>
+      <c r="O124" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M124" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N124">
-        <f t="shared" si="4"/>
-        <v>1021.0229352475681</v>
+        <v>17.036765253270872</v>
       </c>
       <c r="R124" s="9">
         <v>43026</v>
@@ -37195,20 +37701,24 @@
       </c>
       <c r="J125" s="3"/>
       <c r="K125" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L125" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M125" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N125">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L125" s="15">
+        <v>1020.7320327829005</v>
+      </c>
+      <c r="O125" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M125" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N125">
-        <f t="shared" si="4"/>
-        <v>1020.7320327829005</v>
+        <v>6.3940984020089786</v>
       </c>
       <c r="R125" s="9">
         <v>43026</v>
@@ -37491,20 +38001,24 @@
       </c>
       <c r="J126" s="3"/>
       <c r="K126" s="12">
+        <f t="shared" si="7"/>
+        <v>997.40018425598942</v>
+      </c>
+      <c r="L126" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M126" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N126">
         <f t="shared" si="5"/>
-        <v>997.40018425598942</v>
-      </c>
-      <c r="L126" s="15">
+        <v>1020.7320327829005</v>
+      </c>
+      <c r="O126" s="19">
         <f t="shared" si="6"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M126" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N126">
-        <f t="shared" si="4"/>
-        <v>1020.7320327829005</v>
+        <v>5.2846201404731747</v>
       </c>
       <c r="R126" s="9">
         <v>43026</v>
@@ -37789,20 +38303,24 @@
       </c>
       <c r="J127" s="3"/>
       <c r="K127" s="12">
+        <f t="shared" si="7"/>
+        <v>997.27708768547382</v>
+      </c>
+      <c r="L127" s="15">
+        <f t="shared" si="8"/>
+        <v>0.760435858711068</v>
+      </c>
+      <c r="M127" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2180659439999997E-3</v>
+      </c>
+      <c r="N127">
         <f t="shared" si="5"/>
-        <v>997.27708768547382</v>
-      </c>
-      <c r="L127" s="15">
+        <v>1020.9644870534015</v>
+      </c>
+      <c r="O127" s="19">
         <f t="shared" si="6"/>
-        <v>0.760435858711068</v>
-      </c>
-      <c r="M127" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2180659439999997E-3</v>
-      </c>
-      <c r="N127">
-        <f t="shared" si="4"/>
-        <v>1020.9644870534015</v>
+        <v>9.2737370723694514</v>
       </c>
       <c r="R127" s="9">
         <v>43026</v>
@@ -38089,20 +38607,24 @@
       </c>
       <c r="J128" s="3"/>
       <c r="K128" s="12">
+        <f t="shared" si="7"/>
+        <v>997.25217771670884</v>
+      </c>
+      <c r="L128" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M128" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N128">
         <f t="shared" si="5"/>
-        <v>997.25217771670884</v>
-      </c>
-      <c r="L128" s="15">
+        <v>1021.1617293120976</v>
+      </c>
+      <c r="O128" s="19">
         <f t="shared" si="6"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M128" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N128">
-        <f t="shared" si="4"/>
-        <v>1021.1617293120976</v>
+        <v>5.6693979338557385</v>
       </c>
       <c r="R128" s="9">
         <v>43026</v>
@@ -38389,20 +38911,24 @@
       </c>
       <c r="J129" s="3"/>
       <c r="K129" s="12">
+        <f t="shared" si="7"/>
+        <v>997.32661753089724</v>
+      </c>
+      <c r="L129" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M129" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N129">
         <f t="shared" si="5"/>
-        <v>997.32661753089724</v>
-      </c>
-      <c r="L129" s="15">
+        <v>1021.4008023889601</v>
+      </c>
+      <c r="O129" s="19">
         <f t="shared" si="6"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M129" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N129">
-        <f t="shared" si="4"/>
-        <v>1021.4008023889601</v>
+        <v>8.29641663444065</v>
       </c>
       <c r="R129" s="9">
         <v>43026</v>
@@ -38689,20 +39215,24 @@
       </c>
       <c r="J130" s="3"/>
       <c r="K130" s="12">
+        <f t="shared" si="7"/>
+        <v>997.35123703333397</v>
+      </c>
+      <c r="L130" s="15">
+        <f t="shared" si="8"/>
+        <v>0.76089952447632669</v>
+      </c>
+      <c r="M130" s="17">
+        <f t="shared" si="9"/>
+        <v>-4.2248710660000004E-3</v>
+      </c>
+      <c r="N130">
         <f t="shared" si="5"/>
-        <v>997.35123703333397</v>
-      </c>
-      <c r="L130" s="15">
+        <v>1021.3543787243402</v>
+      </c>
+      <c r="O130" s="19">
         <f t="shared" si="6"/>
-        <v>0.76089952447632669</v>
-      </c>
-      <c r="M130" s="17">
-        <f t="shared" si="7"/>
-        <v>-4.2248710660000004E-3</v>
-      </c>
-      <c r="N130">
-        <f t="shared" si="4"/>
-        <v>1021.3543787243402</v>
+        <v>6.3068070796673412</v>
       </c>
       <c r="R130" s="9">
         <v>43026</v>
@@ -38989,20 +39519,24 @@
       </c>
       <c r="J131" s="3"/>
       <c r="K131" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>997.35123703333397</v>
       </c>
       <c r="L131" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.76089952447632669</v>
       </c>
       <c r="M131" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-4.2248710660000004E-3</v>
       </c>
       <c r="N131">
-        <f t="shared" ref="N131:N141" si="8" xml:space="preserve"> K131 + (L131*G131) + M131*G131^(3/2) + 0.00048314*G131^2</f>
+        <f t="shared" ref="N131:N141" si="10" xml:space="preserve"> K131 + (L131*G131) + M131*G131^(3/2) + 0.00048314*G131^2</f>
         <v>1021.3543787243402</v>
+      </c>
+      <c r="O131" s="19">
+        <f t="shared" ref="O131:O141" si="11">I131*(1/     (1-   (0.001*N131/1.84)))</f>
+        <v>8.5993741578072864</v>
       </c>
       <c r="R131" s="9">
         <v>43026</v>
@@ -39289,20 +39823,24 @@
       </c>
       <c r="J132" s="3"/>
       <c r="K132" s="12">
-        <f t="shared" ref="K132:K141" si="9">1000*(1-(F132+288.9414)/(508929.2*(F132+68.12963))*(F132-3.9863)^2)</f>
+        <f t="shared" ref="K132:K141" si="12">1000*(1-(F132+288.9414)/(508929.2*(F132+68.12963))*(F132-3.9863)^2)</f>
         <v>997.27708768547382</v>
       </c>
       <c r="L132" s="15">
-        <f t="shared" ref="L132:L141" si="10" xml:space="preserve"> 0.824493 - 0.0040899*F132 + 0.000076438*F132^2 -0.00000082467*F132^3 + 0.0000000053675*F132^4</f>
+        <f t="shared" ref="L132:L141" si="13" xml:space="preserve"> 0.824493 - 0.0040899*F132 + 0.000076438*F132^2 -0.00000082467*F132^3 + 0.0000000053675*F132^4</f>
         <v>0.760435858711068</v>
       </c>
       <c r="M132" s="17">
-        <f t="shared" ref="M132:M141" si="11" xml:space="preserve"> -0.005724 + 0.00010227*F132 - 0.0000016546*F132^2</f>
+        <f t="shared" ref="M132:M141" si="14" xml:space="preserve"> -0.005724 + 0.00010227*F132 - 0.0000016546*F132^2</f>
         <v>-4.2180659439999997E-3</v>
       </c>
       <c r="N132">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1021.1155677024707</v>
+      </c>
+      <c r="O132" s="19">
+        <f t="shared" si="11"/>
+        <v>1.7638630593421747</v>
       </c>
       <c r="R132" s="9">
         <v>43026</v>
@@ -39587,20 +40125,24 @@
       </c>
       <c r="J133" s="3"/>
       <c r="K133" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>997.35123703333397</v>
       </c>
       <c r="L133" s="15">
+        <f t="shared" si="13"/>
+        <v>0.76089952447632669</v>
+      </c>
+      <c r="M133" s="17">
+        <f t="shared" si="14"/>
+        <v>-4.2248710660000004E-3</v>
+      </c>
+      <c r="N133">
         <f t="shared" si="10"/>
-        <v>0.76089952447632669</v>
-      </c>
-      <c r="M133" s="17">
+        <v>1021.2787876796716</v>
+      </c>
+      <c r="O133" s="19">
         <f t="shared" si="11"/>
-        <v>-4.2248710660000004E-3</v>
-      </c>
-      <c r="N133">
-        <f t="shared" si="8"/>
-        <v>1021.2787876796716</v>
+        <v>7.4748765610406398</v>
       </c>
       <c r="R133" s="9">
         <v>43026</v>
@@ -39883,20 +40425,24 @@
       </c>
       <c r="J134" s="3"/>
       <c r="K134" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L134" s="15">
+        <f t="shared" si="13"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M134" s="17">
+        <f t="shared" si="14"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N134">
         <f t="shared" si="10"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M134" s="17">
+        <v>1021.0985005999307</v>
+      </c>
+      <c r="O134" s="19">
         <f t="shared" si="11"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N134">
-        <f t="shared" si="8"/>
-        <v>1021.0985005999307</v>
+        <v>4.7387384231716698</v>
       </c>
       <c r="R134" s="9">
         <v>43026</v>
@@ -40181,20 +40727,24 @@
       </c>
       <c r="J135" s="3"/>
       <c r="K135" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>997.32661753089724</v>
       </c>
       <c r="L135" s="15">
+        <f t="shared" si="13"/>
+        <v>0.76074425760000008</v>
+      </c>
+      <c r="M135" s="17">
+        <f t="shared" si="14"/>
+        <v>-4.2225696E-3</v>
+      </c>
+      <c r="N135">
         <f t="shared" si="10"/>
-        <v>0.76074425760000008</v>
-      </c>
-      <c r="M135" s="17">
+        <v>1021.0985005999307</v>
+      </c>
+      <c r="O135" s="19">
         <f t="shared" si="11"/>
-        <v>-4.2225696E-3</v>
-      </c>
-      <c r="N135">
-        <f t="shared" si="8"/>
-        <v>1021.0985005999307</v>
+        <v>4.0107387792135754</v>
       </c>
       <c r="R135" s="9">
         <v>43026</v>
@@ -40477,20 +41027,24 @@
       </c>
       <c r="J136" s="3"/>
       <c r="K136" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L136" s="15">
+        <f t="shared" si="13"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M136" s="17">
+        <f t="shared" si="14"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N136">
         <f t="shared" si="10"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M136" s="17">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O136" s="19">
         <f t="shared" si="11"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N136">
-        <f t="shared" si="8"/>
-        <v>1021.2612205430163</v>
+        <v>8.4747909517635751</v>
       </c>
       <c r="R136" s="9">
         <v>43026</v>
@@ -40777,20 +41331,24 @@
       </c>
       <c r="J137" s="3"/>
       <c r="K137" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L137" s="15">
+        <f t="shared" si="13"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M137" s="17">
+        <f t="shared" si="14"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N137">
         <f t="shared" si="10"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M137" s="17">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O137" s="19">
         <f t="shared" si="11"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N137">
-        <f t="shared" si="8"/>
-        <v>1021.2612205430163</v>
+        <v>4.2475085915760165</v>
       </c>
       <c r="R137" s="9">
         <v>43026</v>
@@ -41073,20 +41631,24 @@
       </c>
       <c r="J138" s="3"/>
       <c r="K138" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>997.25217771670884</v>
       </c>
       <c r="L138" s="15">
+        <f t="shared" si="13"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M138" s="17">
+        <f t="shared" si="14"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N138">
         <f t="shared" si="10"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M138" s="17">
+        <v>1021.0861963783011</v>
+      </c>
+      <c r="O138" s="19">
         <f t="shared" si="11"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N138">
-        <f t="shared" si="8"/>
-        <v>1021.0861963783011</v>
+        <v>5.7609970416121987</v>
       </c>
       <c r="R138" s="9">
         <v>43026</v>
@@ -41373,20 +41935,24 @@
       </c>
       <c r="J139" s="3"/>
       <c r="K139" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>997.25217771670884</v>
       </c>
       <c r="L139" s="15">
+        <f t="shared" si="13"/>
+        <v>0.76028272301154676</v>
+      </c>
+      <c r="M139" s="17">
+        <f t="shared" si="14"/>
+        <v>-4.2158637539999998E-3</v>
+      </c>
+      <c r="N139">
         <f t="shared" si="10"/>
-        <v>0.76028272301154676</v>
-      </c>
-      <c r="M139" s="17">
+        <v>1021.0861963783011</v>
+      </c>
+      <c r="O139" s="19">
         <f t="shared" si="11"/>
-        <v>-4.2158637539999998E-3</v>
-      </c>
-      <c r="N139">
-        <f t="shared" si="8"/>
-        <v>1021.0861963783011</v>
+        <v>8.0236039140394553</v>
       </c>
       <c r="R139" s="9">
         <v>43026</v>
@@ -41675,20 +42241,24 @@
       </c>
       <c r="J140" s="3"/>
       <c r="K140" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L140" s="15">
+        <f t="shared" si="13"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M140" s="17">
+        <f t="shared" si="14"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N140">
         <f t="shared" si="10"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M140" s="17">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O140" s="19">
         <f t="shared" si="11"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N140">
-        <f t="shared" si="8"/>
-        <v>1021.2612205430163</v>
+        <v>7.6769784914410959</v>
       </c>
       <c r="R140" s="9">
         <v>43026</v>
@@ -41973,20 +42543,24 @@
       </c>
       <c r="J141" s="3"/>
       <c r="K141" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>997.40018425598942</v>
       </c>
       <c r="L141" s="15">
+        <f t="shared" si="13"/>
+        <v>0.76121220240660681</v>
+      </c>
+      <c r="M141" s="17">
+        <f t="shared" si="14"/>
+        <v>-4.2295732740000001E-3</v>
+      </c>
+      <c r="N141">
         <f t="shared" si="10"/>
-        <v>0.76121220240660681</v>
-      </c>
-      <c r="M141" s="17">
+        <v>1021.2612205430163</v>
+      </c>
+      <c r="O141" s="19">
         <f t="shared" si="11"/>
-        <v>-4.2295732740000001E-3</v>
-      </c>
-      <c r="N141">
-        <f t="shared" si="8"/>
-        <v>1021.2612205430163</v>
+        <v>4.7486696582011234</v>
       </c>
       <c r="R141" s="9">
         <v>43026</v>

</xml_diff>